<commit_message>
Export template ko co active
</commit_message>
<xml_diff>
--- a/DMS/Templates/Product_Export.xlsx
+++ b/DMS/Templates/Product_Export.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FIS\Project\RangDong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdat\OneDrive\Máy tính\Code_RD\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B8C74A-E926-4A16-B71A-7D65BEA66397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{344C91CA-5C39-4A01-8609-C848852C174B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -21,9 +20,7 @@
     <sheet name="UoMGroup" sheetId="8" r:id="rId6"/>
     <sheet name="Supplier" sheetId="9" r:id="rId7"/>
     <sheet name="Brand" sheetId="12" r:id="rId8"/>
-    <sheet name="District" sheetId="11" r:id="rId9"/>
-    <sheet name="Ward" sheetId="10" r:id="rId10"/>
-    <sheet name="Quy tac import" sheetId="5" r:id="rId11"/>
+    <sheet name="Quy tac import" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Linh Cute</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{8F6486FC-21ED-4C66-81E7-306D88CD106F}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{2C6DCBD5-3BA6-4EA0-B1C6-45D9AB2EC447}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{B0A9D51F-52C8-45F9-96C6-9F3E5005DBDC}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{4E8C17C5-503B-4189-A2C3-412D1FEBE87C}">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{F6B9C524-8A37-4004-A660-9FC8F9CA40E0}">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,12 +176,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Linh Cute</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{9A4BBA03-29A1-4D98-A824-4C2ABB82D8A9}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -213,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>STT</t>
   </si>
@@ -307,7 +304,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -317,7 +314,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -349,7 +346,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -360,7 +357,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -376,7 +373,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -386,7 +383,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -422,12 +419,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -435,7 +432,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -454,7 +451,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -870,37 +867,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0C5A16-83ED-4170-9975-2AD2345BC7B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="4"/>
-    <col min="2" max="2" width="12.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="12.21875" style="4" customWidth="1"/>
     <col min="3" max="3" width="27" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.25" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.75" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="4" customWidth="1"/>
-    <col min="7" max="8" width="16.75" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="16.77734375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="13" style="4" customWidth="1"/>
     <col min="12" max="12" width="16" style="4" customWidth="1"/>
-    <col min="13" max="17" width="13.75" style="4" customWidth="1"/>
-    <col min="18" max="18" width="9.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.25" style="4" customWidth="1"/>
+    <col min="13" max="17" width="13.77734375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" style="4" customWidth="1"/>
     <col min="20" max="20" width="10" style="4" customWidth="1"/>
-    <col min="21" max="21" width="12.875" style="4" customWidth="1"/>
-    <col min="22" max="22" width="9.375" style="4" customWidth="1"/>
-    <col min="23" max="23" width="12.625" style="4" customWidth="1"/>
-    <col min="24" max="16384" width="9.125" style="4"/>
+    <col min="21" max="21" width="12.88671875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="9.33203125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" style="4" customWidth="1"/>
+    <col min="24" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -977,7 +974,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="K1:K1048576" xr:uid="{CB885E5D-9D60-4074-BD61-3C06D251CA03}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="K1:K1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -985,19 +982,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" xr:uid="{7441C822-EE58-4EFE-B5A7-AC81319689E6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
           <x14:formula1>
             <xm:f>ProductGroup!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" xr:uid="{19BB5D39-69FE-409D-887A-C661AECA8C65}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
           <x14:formula1>
             <xm:f>ProductType!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" xr:uid="{5C602D6F-254E-47F7-8B5F-F75FD2016E1A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
           <x14:formula1>
             <xm:f>Supplier!#REF!</xm:f>
           </x14:formula1>
@@ -1009,20 +1006,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C99DD-DB6C-4AE7-A7CA-94B6B1380EBF}">
-  <dimension ref="A1:B4"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="15.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1030,37 +1079,194 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3EDC11-6919-41C4-938D-1B041893413C}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="20.625" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1081,7 +1287,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1098,7 +1304,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1115,7 +1321,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1132,7 +1338,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1149,7 +1355,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1166,7 +1372,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1183,7 +1389,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1200,7 +1406,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1217,7 +1423,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1234,7 +1440,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1251,7 +1457,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1268,7 +1474,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1285,7 +1491,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1302,7 +1508,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1319,7 +1525,7 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1336,7 +1542,7 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1353,7 +1559,7 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1370,7 +1576,7 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1387,7 +1593,7 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1404,7 +1610,7 @@
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1421,7 +1627,7 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1438,7 +1644,7 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1455,7 +1661,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -1472,7 +1678,7 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1489,7 +1695,7 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1506,7 +1712,7 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1523,7 +1729,7 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1540,7 +1746,7 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1557,7 +1763,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1574,7 +1780,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1591,7 +1797,7 @@
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1608,7 +1814,7 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1625,7 +1831,7 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1642,7 +1848,7 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1653,7 +1859,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1672,283 +1878,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F55C7FA-359E-480D-BEC4-C9770958DA6B}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.125" style="3"/>
-    <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.75" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF75BD1-B240-4660-99C3-83A30088D35E}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-    <col min="2" max="2" width="19.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE02997-E308-45BB-8AB9-3E5D7DA29A4A}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1CFC51-458A-4BB8-AFAE-92B954E0D1AE}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DA43E8-32C8-40D5-B8CA-89A588E4B9CC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8436F51E-D794-496B-87BC-DC2755C409A0}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F711C948-D32A-43DD-8FC1-DE9DC50E2ADA}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA7963C-C3D0-4ACB-9456-92437D389949}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sửa lại import product
</commit_message>
<xml_diff>
--- a/DMS/Templates/Product_Export.xlsx
+++ b/DMS/Templates/Product_Export.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdat\OneDrive\Máy tính\Code_RD\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C2C39C-7F94-488F-80FD-0242536016E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -38,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Linh Cute</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -145,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -176,12 +177,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Linh Cute</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -210,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -415,11 +416,17 @@
 7. Mặc định trạng thái sau import là Không hoạt động (Status = 0)</t>
     </r>
   </si>
+  <si>
+    <t>% VAT *</t>
+  </si>
+  <si>
+    <t>Có tạo phiên bản*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,6 +560,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,11 +880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -887,17 +900,17 @@
     <col min="10" max="10" width="13.109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="13" style="4" customWidth="1"/>
     <col min="12" max="12" width="16" style="4" customWidth="1"/>
-    <col min="13" max="17" width="13.77734375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="10" style="4" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" style="4" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" style="4" customWidth="1"/>
-    <col min="24" max="16384" width="9.109375" style="4"/>
+    <col min="13" max="19" width="13.77734375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="10" style="4" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="9.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="4" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -937,77 +950,60 @@
       <c r="M1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="K1:K1048576"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" sqref="D1:E1048576 H1:H1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
-          <x14:formula1>
-            <xm:f>ProductGroup!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
-          <x14:formula1>
-            <xm:f>ProductType!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách">
-          <x14:formula1>
-            <xm:f>Supplier!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1058,7 +1054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1086,7 +1082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1113,7 +1109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1143,7 +1139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1179,7 +1175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1215,7 +1211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1251,7 +1247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:Q37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">

</xml_diff>

<commit_message>
thêm category vào product
</commit_message>
<xml_diff>
--- a/DMS/Templates/Product_Export.xlsx
+++ b/DMS/Templates/Product_Export.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B893EBBA-DEF3-47C0-8763-500093393C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9288CF65-C8E9-458E-8591-F11CAC6BF7C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="ProductGroup" sheetId="2" r:id="rId2"/>
-    <sheet name="ProductType" sheetId="6" r:id="rId3"/>
-    <sheet name="UoM" sheetId="7" r:id="rId4"/>
-    <sheet name="UoMGroup" sheetId="8" r:id="rId5"/>
-    <sheet name="Supplier" sheetId="9" r:id="rId6"/>
-    <sheet name="Brand" sheetId="12" r:id="rId7"/>
-    <sheet name="VAT" sheetId="14" r:id="rId8"/>
-    <sheet name="Quy tac import" sheetId="5" r:id="rId9"/>
+    <sheet name="Category" sheetId="15" r:id="rId2"/>
+    <sheet name="ProductGroup" sheetId="2" r:id="rId3"/>
+    <sheet name="ProductType" sheetId="6" r:id="rId4"/>
+    <sheet name="UoM" sheetId="7" r:id="rId5"/>
+    <sheet name="UoMGroup" sheetId="8" r:id="rId6"/>
+    <sheet name="Supplier" sheetId="9" r:id="rId7"/>
+    <sheet name="Brand" sheetId="12" r:id="rId8"/>
+    <sheet name="VAT" sheetId="14" r:id="rId9"/>
+    <sheet name="Quy tac import" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -223,34 +224,19 @@
     <t>Giá bán*</t>
   </si>
   <si>
-    <t>Giá bán lẻ đề xuất</t>
-  </si>
-  <si>
     <t>Trạng thái*</t>
   </si>
   <si>
     <t>Có tạo phiên bản*</t>
   </si>
   <si>
-    <t>Thuộc tính 1</t>
-  </si>
-  <si>
     <t>Giá trị 1</t>
   </si>
   <si>
-    <t>Thuộc tính 2</t>
-  </si>
-  <si>
     <t>Giá trị 2</t>
   </si>
   <si>
-    <t>Thuộc tính 3</t>
-  </si>
-  <si>
     <t>Giá trị 3</t>
-  </si>
-  <si>
-    <t>Thuộc tính 4</t>
   </si>
   <si>
     <t>Giá trị 4</t>
@@ -383,6 +369,36 @@
 6. Import cho đến khi hết dòng có dữ liệu
 7. Trạng thái của sản phẩm phiên bản (item) mặc định bằng trạng thái của sản phẩm (product))</t>
     </r>
+  </si>
+  <si>
+    <t>Danh mục sản phẩm *</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Vui lòng insert vào trên dòng này</t>
+  </si>
+  <si>
+    <t>Nhóm thuộc tính 1</t>
+  </si>
+  <si>
+    <t>Nhóm thuộc tính 2</t>
+  </si>
+  <si>
+    <t>Nhóm thuộc tính 3</t>
+  </si>
+  <si>
+    <t>Nhóm thuộc tính 4</t>
+  </si>
+  <si>
+    <t>Mã danh mục sản phẩm</t>
+  </si>
+  <si>
+    <t>Tên danh mục sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -491,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -516,18 +532,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,39 +873,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="16.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13" style="3" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" customWidth="1"/>
-    <col min="13" max="15" width="13.6640625" style="3" customWidth="1"/>
-    <col min="16" max="18" width="13.6640625" style="4" customWidth="1"/>
-    <col min="19" max="20" width="13.6640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="27" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="3" customWidth="1"/>
+    <col min="8" max="9" width="16.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16" style="3" customWidth="1"/>
+    <col min="14" max="16" width="13.7109375" style="3" customWidth="1"/>
+    <col min="17" max="18" width="13.7109375" style="4" customWidth="1"/>
+    <col min="19" max="20" width="13.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.88671875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" style="1" customWidth="1"/>
-    <col min="27" max="29" width="9.109375" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.109375" style="1"/>
+    <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" style="1" customWidth="1"/>
+    <col min="27" max="29" width="9.140625" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -885,83 +916,147 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="V1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="X1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+    </row>
+    <row r="3" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="K1:K30 K31:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" sqref="H31:H1048576 H1:H30 D1:E30 D31:E1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="L1:L30 L31:L1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Nhập lại" error="Vui lòng chọn giá trị từ danh sách" sqref="I31:I1048576 I1:I30 E1:F30 E31:F1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:S30 S31:S1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Có, Không"</formula1>
     </dataValidation>
@@ -975,210 +1070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.5546875" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="5"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:Q37"/>
   <sheetViews>
@@ -1186,17 +1078,17 @@
       <selection activeCell="B2" sqref="B2:J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1207,7 +1099,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="L2" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -1215,7 +1107,7 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1232,7 +1124,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1249,7 +1141,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1266,7 +1158,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1283,7 +1175,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1300,7 +1192,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1317,7 +1209,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1334,7 +1226,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1351,7 +1243,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1368,7 +1260,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1385,7 +1277,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1402,7 +1294,7 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1419,7 +1311,7 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1436,7 +1328,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1453,7 +1345,7 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1470,7 +1362,7 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1487,7 +1379,7 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1504,7 +1396,7 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1521,7 +1413,7 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1538,7 +1430,7 @@
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1555,7 +1447,7 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1572,7 +1464,7 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1589,7 +1481,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -1606,7 +1498,7 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1623,7 +1515,7 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1640,7 +1532,7 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1657,7 +1549,7 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1674,7 +1566,7 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1691,7 +1583,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1708,7 +1600,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1725,7 +1617,7 @@
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1742,7 +1634,7 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1759,7 +1651,7 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1776,7 +1668,7 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1787,7 +1679,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1806,4 +1698,858 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F4151C-E1DC-496C-801B-62F5439C6250}">
+  <dimension ref="A1:B157"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="20" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="19"/>
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="19"/>
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="19"/>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="19"/>
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="19"/>
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="19"/>
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="19"/>
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="19"/>
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="19"/>
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="19"/>
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="19"/>
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="19"/>
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="19"/>
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="19"/>
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="19"/>
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="19"/>
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="19"/>
+      <c r="B110" s="19"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="19"/>
+      <c r="B111" s="19"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="19"/>
+      <c r="B112" s="19"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="19"/>
+      <c r="B113" s="19"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="19"/>
+      <c r="B114" s="19"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="19"/>
+      <c r="B115" s="19"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="19"/>
+      <c r="B116" s="19"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="19"/>
+      <c r="B117" s="19"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="19"/>
+      <c r="B119" s="19"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="19"/>
+      <c r="B120" s="19"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="19"/>
+      <c r="B121" s="19"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="19"/>
+      <c r="B122" s="19"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="19"/>
+      <c r="B123" s="19"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="19"/>
+      <c r="B124" s="19"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="19"/>
+      <c r="B125" s="19"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="19"/>
+      <c r="B126" s="19"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="19"/>
+      <c r="B127" s="19"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="19"/>
+      <c r="B128" s="19"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="19"/>
+      <c r="B129" s="19"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="19"/>
+      <c r="B130" s="19"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="19"/>
+      <c r="B131" s="19"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="19"/>
+      <c r="B132" s="19"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="19"/>
+      <c r="B133" s="19"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="19"/>
+      <c r="B134" s="19"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="19"/>
+      <c r="B135" s="19"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="19"/>
+      <c r="B136" s="19"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="19"/>
+      <c r="B137" s="19"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="19"/>
+      <c r="B138" s="19"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="19"/>
+      <c r="B139" s="19"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="19"/>
+      <c r="B140" s="19"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="19"/>
+      <c r="B141" s="19"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="19"/>
+      <c r="B142" s="19"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="19"/>
+      <c r="B143" s="19"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="19"/>
+      <c r="B144" s="19"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="19"/>
+      <c r="B145" s="19"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="19"/>
+      <c r="B146" s="19"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="19"/>
+      <c r="B147" s="19"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="19"/>
+      <c r="B148" s="19"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="19"/>
+      <c r="B149" s="19"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="19"/>
+      <c r="B150" s="19"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="19"/>
+      <c r="B151" s="19"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="19"/>
+      <c r="B152" s="19"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="19"/>
+      <c r="B153" s="19"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="19"/>
+      <c r="B154" s="19"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="19"/>
+      <c r="B155" s="19"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="19"/>
+      <c r="B157" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>